<commit_message>
Modified C3 graphics to pull data from external JSON.
</commit_message>
<xml_diff>
--- a/data/UNCCH-tuition-local.xlsx
+++ b/data/UNCCH-tuition-local.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="-1420" windowWidth="31180" windowHeight="21180" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15100" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="44">
   <si>
     <t>2000-2001</t>
   </si>
@@ -171,6 +171,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -279,7 +280,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="64">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -344,8 +345,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -382,7 +390,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="59"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -391,17 +399,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="64">
+  <cellStyles count="71">
     <cellStyle name="Comma" xfId="46" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -435,6 +448,13 @@
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1421,11 +1441,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2143574264"/>
-        <c:axId val="-2143571224"/>
+        <c:axId val="2101512696"/>
+        <c:axId val="2101512328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2143574264"/>
+        <c:axId val="2101512696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1435,7 +1455,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143571224"/>
+        <c:crossAx val="2101512328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1443,7 +1463,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2143571224"/>
+        <c:axId val="2101512328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1454,14 +1474,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143574264"/>
+        <c:crossAx val="2101512696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1762,11 +1781,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2137071224"/>
-        <c:axId val="2137064984"/>
+        <c:axId val="2103104616"/>
+        <c:axId val="2103108312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2137071224"/>
+        <c:axId val="2103104616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1808,7 +1827,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2137064984"/>
+        <c:crossAx val="2103108312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1816,7 +1835,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2137064984"/>
+        <c:axId val="2103108312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1867,7 +1886,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2137071224"/>
+        <c:crossAx val="2103104616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2238,11 +2257,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2144427896"/>
-        <c:axId val="-2144404872"/>
+        <c:axId val="2101421944"/>
+        <c:axId val="2101418248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2144427896"/>
+        <c:axId val="2101421944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2284,7 +2303,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2144404872"/>
+        <c:crossAx val="2101418248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2292,7 +2311,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144404872"/>
+        <c:axId val="2101418248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2343,7 +2362,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2144427896"/>
+        <c:crossAx val="2101421944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6446,10 +6465,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AZ44"/>
+  <dimension ref="A1:BE44"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="BD33" sqref="BD33"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="AX25" sqref="AX25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6474,7 +6493,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="28" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="29" t="s">
@@ -6491,16 +6510,16 @@
       <c r="K1" s="29"/>
       <c r="L1" s="29"/>
       <c r="M1" s="29"/>
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
       <c r="V1" s="29" t="s">
         <v>36</v>
       </c>
@@ -6515,16 +6534,16 @@
       <c r="AE1" s="29"/>
       <c r="AF1" s="29"/>
       <c r="AG1" s="29"/>
-      <c r="AH1" s="28" t="s">
+      <c r="AH1" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="28"/>
-      <c r="AO1" s="28"/>
+      <c r="AI1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
+      <c r="AL1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="32"/>
+      <c r="AO1" s="32"/>
       <c r="AP1" s="29" t="s">
         <v>41</v>
       </c>
@@ -6537,7 +6556,7 @@
       <c r="AW1" s="29"/>
     </row>
     <row r="2" spans="1:49">
-      <c r="A2" s="31"/>
+      <c r="A2" s="28"/>
       <c r="B2" s="30" t="s">
         <v>32</v>
       </c>
@@ -6548,87 +6567,87 @@
       </c>
       <c r="F2" s="33"/>
       <c r="G2" s="33"/>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="31" t="s">
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
       <c r="N2" s="30" t="s">
         <v>32</v>
       </c>
       <c r="O2" s="30"/>
-      <c r="P2" s="31" t="s">
+      <c r="P2" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="32" t="s">
+      <c r="Q2" s="28"/>
+      <c r="R2" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="32"/>
-      <c r="T2" s="31" t="s">
+      <c r="S2" s="31"/>
+      <c r="T2" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="31"/>
+      <c r="U2" s="28"/>
       <c r="V2" s="30" t="s">
         <v>32</v>
       </c>
       <c r="W2" s="30"/>
       <c r="X2" s="30"/>
-      <c r="Y2" s="31" t="s">
+      <c r="Y2" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="Z2" s="31"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="32" t="s">
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="31" t="s">
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="31"/>
+      <c r="AF2" s="28"/>
+      <c r="AG2" s="28"/>
       <c r="AH2" s="30" t="s">
         <v>32</v>
       </c>
       <c r="AI2" s="30"/>
-      <c r="AJ2" s="31" t="s">
+      <c r="AJ2" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="AK2" s="31"/>
-      <c r="AL2" s="32" t="s">
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="31" t="s">
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="AO2" s="31"/>
+      <c r="AO2" s="28"/>
       <c r="AP2" s="30" t="s">
         <v>32</v>
       </c>
       <c r="AQ2" s="30"/>
-      <c r="AR2" s="31" t="s">
+      <c r="AR2" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="AS2" s="31"/>
-      <c r="AT2" s="32" t="s">
+      <c r="AS2" s="28"/>
+      <c r="AT2" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="31" t="s">
+      <c r="AU2" s="31"/>
+      <c r="AV2" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="AW2" s="31"/>
+      <c r="AW2" s="28"/>
     </row>
     <row r="3" spans="1:49">
-      <c r="A3" s="31"/>
+      <c r="A3" s="28"/>
       <c r="B3" s="18" t="s">
         <v>34</v>
       </c>
@@ -6774,7 +6793,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:49" ht="18" hidden="1">
+    <row r="4" spans="1:49" ht="17" hidden="1">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -7302,7 +7321,7 @@
         <v>9.9781468531468534E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:49">
+    <row r="9" spans="1:49" ht="16">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -8358,7 +8377,7 @@
         <v>0.19193761154651975</v>
       </c>
     </row>
-    <row r="17" spans="1:52">
+    <row r="17" spans="1:57">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -8490,7 +8509,7 @@
         <v>0.23374821779507535</v>
       </c>
     </row>
-    <row r="18" spans="1:52">
+    <row r="18" spans="1:57">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -8622,7 +8641,7 @@
         <v>0.24161321241613212</v>
       </c>
     </row>
-    <row r="19" spans="1:52">
+    <row r="19" spans="1:57">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -8753,8 +8772,20 @@
         <f t="shared" si="11"/>
         <v>0.2442537096304917</v>
       </c>
-    </row>
-    <row r="20" spans="1:52">
+      <c r="AZ19" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="BA19" s="30"/>
+      <c r="BB19" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="BC19" s="28"/>
+      <c r="BD19" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE19" s="31"/>
+    </row>
+    <row r="20" spans="1:57">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -8885,14 +8916,98 @@
         <f t="shared" si="11"/>
         <v>0.24385833219598743</v>
       </c>
-    </row>
-    <row r="28" spans="1:52" ht="18">
+      <c r="AZ20" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="BA20" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="BB20" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="BC20" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="BD20" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="BE20" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:57">
+      <c r="AZ21" s="3">
+        <v>0.82106881560810097</v>
+      </c>
+      <c r="BA21" s="3">
+        <v>0.17893118439189906</v>
+      </c>
+      <c r="BB21" s="3">
+        <v>0.69567081011573084</v>
+      </c>
+      <c r="BC21" s="3">
+        <v>0.30432918988426916</v>
+      </c>
+      <c r="BD21" s="3">
+        <v>0.7561416678040126</v>
+      </c>
+      <c r="BE21" s="3">
+        <v>0.24385833219598743</v>
+      </c>
+    </row>
+    <row r="23" spans="1:57">
+      <c r="AI23" s="34"/>
+      <c r="AJ23" s="34"/>
+      <c r="AK23" s="34"/>
+      <c r="AL23" s="34"/>
+      <c r="AM23" s="34"/>
+      <c r="AN23" s="34"/>
+    </row>
+    <row r="24" spans="1:57">
+      <c r="AI24" s="34"/>
+      <c r="AJ24" s="34"/>
+      <c r="AK24" s="34"/>
+      <c r="AL24" s="34"/>
+      <c r="AM24" s="34"/>
+      <c r="AN24" s="34"/>
+    </row>
+    <row r="25" spans="1:57">
+      <c r="AI25" s="34"/>
+      <c r="AJ25" s="34"/>
+      <c r="AK25" s="34"/>
+      <c r="AL25" s="34"/>
+      <c r="AM25" s="34"/>
+      <c r="AN25" s="34"/>
+    </row>
+    <row r="26" spans="1:57">
+      <c r="AI26" s="35"/>
+      <c r="AJ26" s="35"/>
+      <c r="AK26" s="35"/>
+      <c r="AL26" s="35"/>
+      <c r="AM26" s="35"/>
+      <c r="AN26" s="35"/>
+    </row>
+    <row r="27" spans="1:57">
+      <c r="AI27" s="34"/>
+      <c r="AJ27" s="34"/>
+      <c r="AK27" s="34"/>
+      <c r="AL27" s="34"/>
+      <c r="AM27" s="34"/>
+      <c r="AN27" s="34"/>
+    </row>
+    <row r="28" spans="1:57" ht="17">
       <c r="O28" s="20"/>
+      <c r="AI28" s="36"/>
+      <c r="AJ28" s="36"/>
+      <c r="AK28" s="36"/>
+      <c r="AL28" s="36"/>
+      <c r="AM28" s="36"/>
+      <c r="AN28" s="36"/>
       <c r="AX28" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:52">
+    <row r="29" spans="1:57">
       <c r="AX29" s="18" t="s">
         <v>32</v>
       </c>
@@ -8903,7 +9018,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:52" ht="16">
+    <row r="30" spans="1:57" ht="16">
       <c r="E30" s="25"/>
       <c r="F30" s="26"/>
       <c r="G30" s="26"/>
@@ -8917,7 +9032,7 @@
         <v>0.26192506916882274</v>
       </c>
     </row>
-    <row r="31" spans="1:52" ht="16">
+    <row r="31" spans="1:57" ht="16">
       <c r="E31" s="25"/>
       <c r="F31" s="26"/>
       <c r="G31" s="26"/>
@@ -8934,7 +9049,7 @@
         <v>0.24678900252380159</v>
       </c>
     </row>
-    <row r="32" spans="1:52" ht="16">
+    <row r="32" spans="1:57" ht="16">
       <c r="E32" s="25"/>
       <c r="F32" s="26"/>
       <c r="G32" s="26"/>
@@ -9177,7 +9292,23 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="32">
+    <mergeCell ref="BD19:BE19"/>
+    <mergeCell ref="AI26:AJ26"/>
+    <mergeCell ref="AK26:AL26"/>
+    <mergeCell ref="AM26:AN26"/>
+    <mergeCell ref="AZ19:BA19"/>
+    <mergeCell ref="BB19:BC19"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:AG1"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="AP1:AW1"/>
     <mergeCell ref="AP2:AQ2"/>
@@ -9194,16 +9325,6 @@
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:AG1"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="AB2:AD2"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Prepared spreadsheet for sharing on portfolio site.
</commit_message>
<xml_diff>
--- a/data/UNCCH-tuition-local.xlsx
+++ b/data/UNCCH-tuition-local.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="43">
   <si>
     <t>2000-2001</t>
   </si>
@@ -153,9 +153,6 @@
   <si>
     <t xml:space="preserve">Percentage of Enrollment </t>
   </si>
-  <si>
-    <t>Percentage of Tuition Revenue</t>
-  </si>
 </sst>
 </file>
 
@@ -165,13 +162,12 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -226,8 +222,19 @@
       <color rgb="FF4C4C4C"/>
       <name val="Lucida Grande"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,6 +277,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -280,7 +293,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -352,8 +365,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -390,31 +407,35 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="59"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="75">
     <cellStyle name="Comma" xfId="46" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -455,6 +476,10 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1441,11 +1466,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2101512696"/>
-        <c:axId val="2101512328"/>
+        <c:axId val="2139255832"/>
+        <c:axId val="2139252792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2101512696"/>
+        <c:axId val="2139255832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1455,7 +1480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101512328"/>
+        <c:crossAx val="2139252792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1463,7 +1488,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2101512328"/>
+        <c:axId val="2139252792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1474,7 +1499,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101512696"/>
+        <c:crossAx val="2139255832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1781,11 +1806,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2103104616"/>
-        <c:axId val="2103108312"/>
+        <c:axId val="2140619272"/>
+        <c:axId val="2140615576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2103104616"/>
+        <c:axId val="2140619272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1827,7 +1852,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2103108312"/>
+        <c:crossAx val="2140615576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1835,7 +1860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2103108312"/>
+        <c:axId val="2140615576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1886,483 +1911,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2103104616"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Percentage of Total Tuition Revenue</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Generate by Out-of-State Students</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$AX$28:$AX$29</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Percentage of Tuition Revenue UNC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$AX$30:$AX$41</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0.458092342278346</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.456317109479905</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.454404873138528</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.466675847471158</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.489623393875792</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.47390653258829</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.480643584569066</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.468197732001741</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.463494212654262</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.490294381570136</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.474749760566722</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.455508026261416</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$AY$28:$AY$29</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Percentage of Tuition Revenue UVA</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$AY$30:$AY$41</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0.586831961554626</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.62142177664071</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.61594260376646</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.610971160358568</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.625467773860333</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.611017671784923</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.603568067541653</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.61200533861594</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.610441028420086</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.613910464285981</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.594609133895886</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.554206328862783</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet2!$AZ$28:$AZ$29</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Percentage of Tuition Revenue Berkeley</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet2!$AZ$30:$AZ$41</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0.261925069168823</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.246789002523802</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.242171717585949</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.25189891935541</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.265304367221101</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.291440902808585</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.343906405430386</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.375061233547191</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.432962575399429</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.440864793751977</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.447817132411741</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.457832375151591</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="2101421944"/>
-        <c:axId val="2101418248"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="2101421944"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2101418248"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2101418248"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2101421944"/>
+        <c:crossAx val="2140619272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2483,563 +2032,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3622,36 +2615,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>49</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Chart 10"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6465,10 +5428,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE44"/>
+  <dimension ref="A1:BE53"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="AX25" sqref="AX25"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="AY28" sqref="AY28:BD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6490,164 +5453,167 @@
     <col min="44" max="45" width="10.83203125" customWidth="1"/>
     <col min="48" max="49" width="0" hidden="1" customWidth="1"/>
     <col min="50" max="50" width="26" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="11.6640625" customWidth="1"/>
+    <col min="54" max="54" width="8.6640625" customWidth="1"/>
+    <col min="55" max="55" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="32" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="29" t="s">
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="29"/>
-      <c r="AG1" s="29"/>
-      <c r="AH1" s="32" t="s">
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="39"/>
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="39"/>
+      <c r="AD1" s="39"/>
+      <c r="AE1" s="39"/>
+      <c r="AF1" s="39"/>
+      <c r="AG1" s="39"/>
+      <c r="AH1" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="29" t="s">
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="38"/>
+      <c r="AN1" s="38"/>
+      <c r="AO1" s="38"/>
+      <c r="AP1" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="29"/>
-      <c r="AR1" s="29"/>
-      <c r="AS1" s="29"/>
-      <c r="AT1" s="29"/>
-      <c r="AU1" s="29"/>
-      <c r="AV1" s="29"/>
-      <c r="AW1" s="29"/>
+      <c r="AQ1" s="39"/>
+      <c r="AR1" s="39"/>
+      <c r="AS1" s="39"/>
+      <c r="AT1" s="39"/>
+      <c r="AU1" s="39"/>
+      <c r="AV1" s="39"/>
+      <c r="AW1" s="39"/>
     </row>
     <row r="2" spans="1:49">
-      <c r="A2" s="28"/>
-      <c r="B2" s="30" t="s">
+      <c r="A2" s="37"/>
+      <c r="B2" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="33" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="31" t="s">
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="28" t="s">
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="30" t="s">
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="28" t="s">
+      <c r="O2" s="36"/>
+      <c r="P2" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="31" t="s">
+      <c r="Q2" s="37"/>
+      <c r="R2" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="31"/>
-      <c r="T2" s="28" t="s">
+      <c r="S2" s="34"/>
+      <c r="T2" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="28"/>
-      <c r="V2" s="30" t="s">
+      <c r="U2" s="37"/>
+      <c r="V2" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="28" t="s">
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Z2" s="28"/>
-      <c r="AA2" s="28"/>
-      <c r="AB2" s="31" t="s">
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="28" t="s">
+      <c r="AC2" s="34"/>
+      <c r="AD2" s="34"/>
+      <c r="AE2" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="AF2" s="28"/>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="30" t="s">
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="37"/>
+      <c r="AH2" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" s="30"/>
-      <c r="AJ2" s="28" t="s">
+      <c r="AI2" s="36"/>
+      <c r="AJ2" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="AK2" s="28"/>
-      <c r="AL2" s="31" t="s">
+      <c r="AK2" s="37"/>
+      <c r="AL2" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="AM2" s="31"/>
-      <c r="AN2" s="28" t="s">
+      <c r="AM2" s="34"/>
+      <c r="AN2" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="AO2" s="28"/>
-      <c r="AP2" s="30" t="s">
+      <c r="AO2" s="37"/>
+      <c r="AP2" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="AQ2" s="30"/>
-      <c r="AR2" s="28" t="s">
+      <c r="AQ2" s="36"/>
+      <c r="AR2" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="AS2" s="28"/>
-      <c r="AT2" s="31" t="s">
+      <c r="AS2" s="37"/>
+      <c r="AT2" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="AU2" s="31"/>
-      <c r="AV2" s="28" t="s">
+      <c r="AU2" s="34"/>
+      <c r="AV2" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="AW2" s="28"/>
+      <c r="AW2" s="37"/>
     </row>
     <row r="3" spans="1:49">
-      <c r="A3" s="28"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="18" t="s">
         <v>34</v>
       </c>
@@ -8772,18 +7738,18 @@
         <f t="shared" si="11"/>
         <v>0.2442537096304917</v>
       </c>
-      <c r="AZ19" s="30" t="s">
+      <c r="AZ19" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="BA19" s="30"/>
-      <c r="BB19" s="28" t="s">
+      <c r="BA19" s="36"/>
+      <c r="BB19" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="BC19" s="28"/>
-      <c r="BD19" s="31" t="s">
+      <c r="BC19" s="37"/>
+      <c r="BD19" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="BE19" s="31"/>
+      <c r="BE19" s="34"/>
     </row>
     <row r="20" spans="1:57">
       <c r="A20" t="s">
@@ -8956,28 +7922,28 @@
       </c>
     </row>
     <row r="23" spans="1:57">
-      <c r="AI23" s="34"/>
-      <c r="AJ23" s="34"/>
-      <c r="AK23" s="34"/>
-      <c r="AL23" s="34"/>
-      <c r="AM23" s="34"/>
-      <c r="AN23" s="34"/>
+      <c r="AI23" s="28"/>
+      <c r="AJ23" s="28"/>
+      <c r="AK23" s="28"/>
+      <c r="AL23" s="28"/>
+      <c r="AM23" s="28"/>
+      <c r="AN23" s="28"/>
     </row>
     <row r="24" spans="1:57">
-      <c r="AI24" s="34"/>
-      <c r="AJ24" s="34"/>
-      <c r="AK24" s="34"/>
-      <c r="AL24" s="34"/>
-      <c r="AM24" s="34"/>
-      <c r="AN24" s="34"/>
+      <c r="AI24" s="28"/>
+      <c r="AJ24" s="28"/>
+      <c r="AK24" s="28"/>
+      <c r="AL24" s="28"/>
+      <c r="AM24" s="28"/>
+      <c r="AN24" s="28"/>
     </row>
     <row r="25" spans="1:57">
-      <c r="AI25" s="34"/>
-      <c r="AJ25" s="34"/>
-      <c r="AK25" s="34"/>
-      <c r="AL25" s="34"/>
-      <c r="AM25" s="34"/>
-      <c r="AN25" s="34"/>
+      <c r="AI25" s="28"/>
+      <c r="AJ25" s="28"/>
+      <c r="AK25" s="28"/>
+      <c r="AL25" s="28"/>
+      <c r="AM25" s="28"/>
+      <c r="AN25" s="28"/>
     </row>
     <row r="26" spans="1:57">
       <c r="AI26" s="35"/>
@@ -8988,49 +7954,32 @@
       <c r="AN26" s="35"/>
     </row>
     <row r="27" spans="1:57">
-      <c r="AI27" s="34"/>
-      <c r="AJ27" s="34"/>
-      <c r="AK27" s="34"/>
-      <c r="AL27" s="34"/>
-      <c r="AM27" s="34"/>
-      <c r="AN27" s="34"/>
+      <c r="AI27" s="28"/>
+      <c r="AJ27" s="28"/>
+      <c r="AK27" s="28"/>
+      <c r="AL27" s="28"/>
+      <c r="AM27" s="28"/>
+      <c r="AN27" s="28"/>
     </row>
     <row r="28" spans="1:57" ht="17">
       <c r="O28" s="20"/>
-      <c r="AI28" s="36"/>
-      <c r="AJ28" s="36"/>
-      <c r="AK28" s="36"/>
-      <c r="AL28" s="36"/>
-      <c r="AM28" s="36"/>
-      <c r="AN28" s="36"/>
-      <c r="AX28" t="s">
-        <v>43</v>
-      </c>
+      <c r="AI28" s="29"/>
+      <c r="AJ28" s="29"/>
+      <c r="AK28" s="29"/>
+      <c r="AL28" s="29"/>
+      <c r="AM28" s="29"/>
+      <c r="AN28" s="29"/>
     </row>
     <row r="29" spans="1:57">
-      <c r="AX29" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="AY29" t="s">
-        <v>33</v>
-      </c>
-      <c r="AZ29" t="s">
-        <v>38</v>
-      </c>
+      <c r="BA29" s="18"/>
     </row>
     <row r="30" spans="1:57" ht="16">
       <c r="E30" s="25"/>
       <c r="F30" s="26"/>
       <c r="G30" s="26"/>
-      <c r="AX30" s="14">
-        <v>0.45809234227834555</v>
-      </c>
-      <c r="AY30" s="3">
-        <v>0.58683196155462591</v>
-      </c>
-      <c r="AZ30" s="3">
-        <v>0.26192506916882274</v>
-      </c>
+      <c r="BA30" s="14"/>
+      <c r="BB30" s="3"/>
+      <c r="BC30" s="3"/>
     </row>
     <row r="31" spans="1:57" ht="16">
       <c r="E31" s="25"/>
@@ -9039,15 +7988,9 @@
       <c r="W31" t="s">
         <v>42</v>
       </c>
-      <c r="AX31" s="14">
-        <v>0.45631710947990539</v>
-      </c>
-      <c r="AY31" s="3">
-        <v>0.62142177664070997</v>
-      </c>
-      <c r="AZ31" s="3">
-        <v>0.24678900252380159</v>
-      </c>
+      <c r="BA31" s="14"/>
+      <c r="BB31" s="3"/>
+      <c r="BC31" s="3"/>
     </row>
     <row r="32" spans="1:57" ht="16">
       <c r="E32" s="25"/>
@@ -9062,17 +8005,11 @@
       <c r="Y32" t="s">
         <v>38</v>
       </c>
-      <c r="AX32" s="14">
-        <v>0.45440487313852768</v>
-      </c>
-      <c r="AY32" s="3">
-        <v>0.61594260376646026</v>
-      </c>
-      <c r="AZ32" s="3">
-        <v>0.24217171758594896</v>
-      </c>
-    </row>
-    <row r="33" spans="5:52" ht="16">
+      <c r="BA32" s="14"/>
+      <c r="BB32" s="3"/>
+      <c r="BC32" s="3"/>
+    </row>
+    <row r="33" spans="5:55" ht="16">
       <c r="E33" s="25"/>
       <c r="F33" s="26"/>
       <c r="G33" s="26"/>
@@ -9085,17 +8022,11 @@
       <c r="Y33" s="3">
         <v>9.4583084916105953E-2</v>
       </c>
-      <c r="AX33" s="14">
-        <v>0.46667584747115842</v>
-      </c>
-      <c r="AY33" s="3">
-        <v>0.61097116035856824</v>
-      </c>
-      <c r="AZ33" s="3">
-        <v>0.25189891935540981</v>
-      </c>
-    </row>
-    <row r="34" spans="5:52" ht="16">
+      <c r="BA33" s="14"/>
+      <c r="BB33" s="3"/>
+      <c r="BC33" s="3"/>
+    </row>
+    <row r="34" spans="5:55" ht="16">
       <c r="E34" s="25"/>
       <c r="F34" s="26"/>
       <c r="G34" s="26"/>
@@ -9108,17 +8039,11 @@
       <c r="Y34" s="3">
         <v>8.8002346729246117E-2</v>
       </c>
-      <c r="AX34" s="14">
-        <v>0.48962339387579235</v>
-      </c>
-      <c r="AY34" s="3">
-        <v>0.62546777386033281</v>
-      </c>
-      <c r="AZ34" s="3">
-        <v>0.26530436722110062</v>
-      </c>
-    </row>
-    <row r="35" spans="5:52">
+      <c r="BA34" s="14"/>
+      <c r="BB34" s="3"/>
+      <c r="BC34" s="3"/>
+    </row>
+    <row r="35" spans="5:55">
       <c r="W35" s="14">
         <v>0.17485331098072088</v>
       </c>
@@ -9128,17 +8053,11 @@
       <c r="Y35" s="3">
         <v>8.7311251826595229E-2</v>
       </c>
-      <c r="AX35" s="14">
-        <v>0.47390653258829013</v>
-      </c>
-      <c r="AY35" s="3">
-        <v>0.61101767178492317</v>
-      </c>
-      <c r="AZ35" s="3">
-        <v>0.29144090280858503</v>
-      </c>
-    </row>
-    <row r="36" spans="5:52">
+      <c r="BA35" s="14"/>
+      <c r="BB35" s="3"/>
+      <c r="BC35" s="3"/>
+    </row>
+    <row r="36" spans="5:55">
       <c r="W36" s="14">
         <v>0.1747956175963517</v>
       </c>
@@ -9148,17 +8067,11 @@
       <c r="Y36" s="27">
         <v>9.2401892568883939E-2</v>
       </c>
-      <c r="AX36" s="14">
-        <v>0.48064358456906631</v>
-      </c>
-      <c r="AY36" s="3">
-        <v>0.60356806754165282</v>
-      </c>
-      <c r="AZ36" s="3">
-        <v>0.34390640543038581</v>
-      </c>
-    </row>
-    <row r="37" spans="5:52">
+      <c r="BA36" s="14"/>
+      <c r="BB36" s="3"/>
+      <c r="BC36" s="3"/>
+    </row>
+    <row r="37" spans="5:55">
       <c r="W37" s="14">
         <v>0.18666236072985629</v>
       </c>
@@ -9168,17 +8081,11 @@
       <c r="Y37" s="3">
         <v>0.10144927536231885</v>
       </c>
-      <c r="AX37" s="14">
-        <v>0.46819773200174103</v>
-      </c>
-      <c r="AY37" s="3">
-        <v>0.61200533861594031</v>
-      </c>
-      <c r="AZ37" s="3">
-        <v>0.37506123354719134</v>
-      </c>
-    </row>
-    <row r="38" spans="5:52">
+      <c r="BA37" s="14"/>
+      <c r="BB37" s="3"/>
+      <c r="BC37" s="3"/>
+    </row>
+    <row r="38" spans="5:55">
       <c r="W38" s="14">
         <v>0.1919153553988063</v>
       </c>
@@ -9188,17 +8095,11 @@
       <c r="Y38" s="3">
         <v>0.12666405638214565</v>
       </c>
-      <c r="AX38" s="14">
-        <v>0.46349421265426177</v>
-      </c>
-      <c r="AY38" s="3">
-        <v>0.61044102842008585</v>
-      </c>
-      <c r="AZ38" s="3">
-        <v>0.43296257539942906</v>
-      </c>
-    </row>
-    <row r="39" spans="5:52">
+      <c r="BA38" s="14"/>
+      <c r="BB38" s="3"/>
+      <c r="BC38" s="3"/>
+    </row>
+    <row r="39" spans="5:55">
       <c r="W39" s="14">
         <v>0.1946711344106361</v>
       </c>
@@ -9208,17 +8109,11 @@
       <c r="Y39" s="3">
         <v>0.1687463782113193</v>
       </c>
-      <c r="AX39" s="14">
-        <v>0.49029438157013605</v>
-      </c>
-      <c r="AY39" s="3">
-        <v>0.61391046428598128</v>
-      </c>
-      <c r="AZ39" s="3">
-        <v>0.44086479375197685</v>
-      </c>
-    </row>
-    <row r="40" spans="5:52">
+      <c r="BA39" s="14"/>
+      <c r="BB39" s="3"/>
+      <c r="BC39" s="3"/>
+    </row>
+    <row r="40" spans="5:55">
       <c r="W40" s="14">
         <v>0.19227000544365813</v>
       </c>
@@ -9228,17 +8123,11 @@
       <c r="Y40" s="3">
         <v>0.19193761154651975</v>
       </c>
-      <c r="AX40" s="14">
-        <v>0.47474976056672163</v>
-      </c>
-      <c r="AY40" s="3">
-        <v>0.5946091338958861</v>
-      </c>
-      <c r="AZ40" s="3">
-        <v>0.44781713241174109</v>
-      </c>
-    </row>
-    <row r="41" spans="5:52">
+      <c r="BA40" s="14"/>
+      <c r="BB40" s="3"/>
+      <c r="BC40" s="3"/>
+    </row>
+    <row r="41" spans="5:55">
       <c r="W41" s="14">
         <v>0.19302452316076293</v>
       </c>
@@ -9248,17 +8137,11 @@
       <c r="Y41" s="3">
         <v>0.23374821779507535</v>
       </c>
-      <c r="AX41" s="14">
-        <v>0.45550802626141568</v>
-      </c>
-      <c r="AY41" s="3">
-        <v>0.55420632886278287</v>
-      </c>
-      <c r="AZ41" s="3">
-        <v>0.45783237515159092</v>
-      </c>
-    </row>
-    <row r="42" spans="5:52">
+      <c r="BA41" s="14"/>
+      <c r="BB41" s="3"/>
+      <c r="BC41" s="3"/>
+    </row>
+    <row r="42" spans="5:55">
       <c r="W42" s="14">
         <v>0.19245180559326636</v>
       </c>
@@ -9269,7 +8152,7 @@
         <v>0.24161321241613212</v>
       </c>
     </row>
-    <row r="43" spans="5:52">
+    <row r="43" spans="5:55">
       <c r="W43" s="14">
         <v>0.187388651946229</v>
       </c>
@@ -9280,7 +8163,7 @@
         <v>0.2442537096304917</v>
       </c>
     </row>
-    <row r="44" spans="5:52">
+    <row r="44" spans="5:55">
       <c r="W44" s="14">
         <v>0.17893118439189906</v>
       </c>
@@ -9291,24 +8174,45 @@
         <v>0.24385833219598743</v>
       </c>
     </row>
+    <row r="47" spans="5:55">
+      <c r="AY47" s="32"/>
+      <c r="AZ47" s="32"/>
+      <c r="BA47" s="32"/>
+    </row>
+    <row r="48" spans="5:55" ht="16">
+      <c r="AY48" s="32"/>
+      <c r="AZ48" s="32"/>
+      <c r="BA48" s="32"/>
+      <c r="BC48" s="30"/>
+    </row>
+    <row r="49" spans="51:55">
+      <c r="AY49" s="32"/>
+      <c r="AZ49" s="33"/>
+      <c r="BA49" s="32"/>
+    </row>
+    <row r="50" spans="51:55">
+      <c r="AY50" s="32"/>
+      <c r="AZ50" s="32"/>
+      <c r="BA50" s="32"/>
+    </row>
+    <row r="51" spans="51:55">
+      <c r="AY51" s="32"/>
+      <c r="AZ51" s="33"/>
+      <c r="BA51" s="32"/>
+    </row>
+    <row r="52" spans="51:55" ht="16">
+      <c r="AY52" s="32"/>
+      <c r="AZ52" s="32"/>
+      <c r="BA52" s="32"/>
+      <c r="BC52" s="31"/>
+    </row>
+    <row r="53" spans="51:55">
+      <c r="AY53" s="32"/>
+      <c r="AZ53" s="32"/>
+      <c r="BA53" s="32"/>
+    </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="BD19:BE19"/>
-    <mergeCell ref="AI26:AJ26"/>
-    <mergeCell ref="AK26:AL26"/>
-    <mergeCell ref="AM26:AN26"/>
-    <mergeCell ref="AZ19:BA19"/>
-    <mergeCell ref="BB19:BC19"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="V1:AG1"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="AB2:AD2"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="AP1:AW1"/>
     <mergeCell ref="AP2:AQ2"/>
@@ -9325,6 +8229,22 @@
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="V1:AG1"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="BD19:BE19"/>
+    <mergeCell ref="AI26:AJ26"/>
+    <mergeCell ref="AK26:AL26"/>
+    <mergeCell ref="AM26:AN26"/>
+    <mergeCell ref="AZ19:BA19"/>
+    <mergeCell ref="BB19:BC19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>